<commit_message>
MB Subset Vendors Taxonomy completed
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/TaxonomyModuleTest.xlsx
+++ b/resources/ExcelsheetData/TaxonomyModuleTest.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="16" activeTab="20"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="createTaxonomy" sheetId="2" r:id="rId2"/>
     <sheet name="createCategories" sheetId="3" r:id="rId3"/>
     <sheet name="createChildCategories" sheetId="4" r:id="rId4"/>
-    <sheet name="verifyEditTaxonomyForm" sheetId="5" r:id="rId5"/>
-    <sheet name="verifyCategoriesInTaxonomyPage" sheetId="6" r:id="rId6"/>
-    <sheet name="verifyTreeCollapsingFeature" sheetId="7" r:id="rId7"/>
-    <sheet name="verifyCategoryDetailsForm" sheetId="8" r:id="rId8"/>
-    <sheet name="verifyCharLimitInCatDescFields" sheetId="9" r:id="rId9"/>
-    <sheet name="verifyCharLimitInMarDescFields" sheetId="11" r:id="rId10"/>
-    <sheet name="verifyChildCategoryFields" sheetId="10" r:id="rId11"/>
+    <sheet name="TC_TaxMgt_011" sheetId="5" r:id="rId5"/>
+    <sheet name="TC_TaxMgt_015" sheetId="6" r:id="rId6"/>
+    <sheet name="TC_TaxMgt_017" sheetId="7" r:id="rId7"/>
+    <sheet name="TC_TaxMgt_019" sheetId="8" r:id="rId8"/>
+    <sheet name="TC_TaxMgt_027" sheetId="9" r:id="rId9"/>
+    <sheet name="TC_TaxMgt_028" sheetId="11" r:id="rId10"/>
+    <sheet name="TC_TaxMgt_029" sheetId="10" r:id="rId11"/>
     <sheet name="TC_TaxMgt_39" sheetId="12" r:id="rId12"/>
     <sheet name="TC_TaxMgt_39_1" sheetId="13" r:id="rId13"/>
     <sheet name="TC_TaxMgt_40" sheetId="14" r:id="rId14"/>
@@ -28,13 +28,36 @@
     <sheet name="TC_TaxMgt_52" sheetId="19" r:id="rId19"/>
     <sheet name="TC_TaxMgt_52_1" sheetId="20" r:id="rId20"/>
     <sheet name="TC_TaxMgt_54" sheetId="21" r:id="rId21"/>
+    <sheet name="TC_TaxMgt_60" sheetId="22" r:id="rId22"/>
+    <sheet name="TC_TaxMgt_62" sheetId="23" r:id="rId23"/>
+    <sheet name="TC_TaxMgt_64" sheetId="24" r:id="rId24"/>
+    <sheet name="TC_TaxMgt_65" sheetId="25" r:id="rId25"/>
+    <sheet name="TC_TaxMgt_66" sheetId="26" r:id="rId26"/>
+    <sheet name="TC_TaxMgt_67" sheetId="27" r:id="rId27"/>
+    <sheet name="TC_TaxMgt_68" sheetId="28" r:id="rId28"/>
+    <sheet name="TC_TaxMgt_69" sheetId="29" r:id="rId29"/>
+    <sheet name="TC_TaxMgt_70" sheetId="30" r:id="rId30"/>
+    <sheet name="TC_TaxMgt_71" sheetId="31" r:id="rId31"/>
+    <sheet name="TC_TaxMgt_74" sheetId="32" r:id="rId32"/>
+    <sheet name="TC_TaxMgt_75" sheetId="33" r:id="rId33"/>
+    <sheet name="TC_TaxMgt_76" sheetId="34" r:id="rId34"/>
+    <sheet name="TC_TaxMgt_77" sheetId="35" r:id="rId35"/>
+    <sheet name="TC_TaxMgt_78" sheetId="36" r:id="rId36"/>
+    <sheet name="TC_TaxMgt_81" sheetId="37" r:id="rId37"/>
+    <sheet name="TC_TaxMgt_84" sheetId="38" r:id="rId38"/>
+    <sheet name="TC_TaxMgt_85" sheetId="39" r:id="rId39"/>
+    <sheet name="TC_TaxMgt_79" sheetId="40" r:id="rId40"/>
+    <sheet name="TC_TaxMgt_94" sheetId="41" r:id="rId41"/>
+    <sheet name="TC_TaxMgt_95" sheetId="42" r:id="rId42"/>
+    <sheet name="TC_TaxMgt_96" sheetId="43" r:id="rId43"/>
+    <sheet name="TC_TaxMgt_97" sheetId="44" r:id="rId44"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="112">
   <si>
     <t>Module Name</t>
   </si>
@@ -324,12 +347,60 @@
   <si>
     <t>1002003</t>
   </si>
+  <si>
+    <t>Attribute Name</t>
+  </si>
+  <si>
+    <t>Attribute Desc</t>
+  </si>
+  <si>
+    <t>ASFASFASF</t>
+  </si>
+  <si>
+    <t>Attribute Name Required</t>
+  </si>
+  <si>
+    <t>TestAttribute1</t>
+  </si>
+  <si>
+    <t>Attribute saved Successfully</t>
+  </si>
+  <si>
+    <t>Edit Attribute  Name</t>
+  </si>
+  <si>
+    <t>TestAttribute123</t>
+  </si>
+  <si>
+    <t>Attribute Group Name</t>
+  </si>
+  <si>
+    <t>Attribute Group Desc</t>
+  </si>
+  <si>
+    <t>Test Attribute Group</t>
+  </si>
+  <si>
+    <t>Attribute Group Name Required</t>
+  </si>
+  <si>
+    <t>Attribute Group saved Successfully</t>
+  </si>
+  <si>
+    <t>Edited Attribute Group Name</t>
+  </si>
+  <si>
+    <t>Edited Attribute Group Desc</t>
+  </si>
+  <si>
+    <t>Test Attribute Group123</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +418,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF696969"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -393,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -418,6 +496,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,7 +832,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,8 +867,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,7 +1459,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,6 +1622,333 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
@@ -1550,7 +1957,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -1634,6 +2041,493 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
@@ -1642,7 +2536,7 @@
       <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -1946,12 +2840,277 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,7 +3194,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="A1:XFD1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2057,13 +3216,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2077,7 +3236,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2120,10 +3279,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+      <selection activeCell="I37" sqref="I37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
updated excelsheet for AdvancedSearchTest
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/TaxonomyModuleTest.xlsx
+++ b/resources/ExcelsheetData/TaxonomyModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23160" windowHeight="4905" firstSheet="34" activeTab="41"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,6 @@
     <sheet name="TC_TaxMgt_97" sheetId="44" r:id="rId44"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:U14"/>
 </workbook>
 </file>
 
@@ -1378,7 +1377,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,7 +1983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -3030,8 +3029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3060,7 +3059,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>